<commit_message>
Added subrecipient tests and cleaned up the fixtures for the other tests to only trigger the intended error
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/data-certification/EOHHS-075-09302020-no-reviewer-v1.xlsx
+++ b/tests/server/fixtures/data-certification/EOHHS-075-09302020-no-reviewer-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/usdr/cares-reporter/tests/server/fixtures/data-certification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5518A3-9A9D-3D45-9D0B-CF883790CBA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A92F878-3B15-8242-9385-54BAA436E320}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certification" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="345">
   <si>
     <t>Certification</t>
   </si>
@@ -1081,6 +1081,9 @@
   <si>
     <t>CRF Project TOTALS</t>
   </si>
+  <si>
+    <t>A category</t>
+  </si>
 </sst>
 </file>
 
@@ -1091,7 +1094,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1150,6 +1153,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1360,7 +1369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1443,6 +1452,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7930,7 +7940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -12921,7 +12931,7 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
@@ -20095,7 +20105,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AY1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AN3" sqref="AN3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -20402,6 +20414,9 @@
         <v>9199.25</v>
       </c>
       <c r="AE3" s="14"/>
+      <c r="AN3" s="54" t="s">
+        <v>344</v>
+      </c>
       <c r="AO3" s="33">
         <v>10000</v>
       </c>
@@ -22947,7 +22962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AR1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="L1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -27688,7 +27703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="N1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -30214,7 +30229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
Separate subrecipients from documents (#188)
* Filter documents (#176)

* UI subrecipient count now coming from API, not documents table

* Moved UI Subrecipients table from Spreadsheet Data dropdown to its own tab

* Minor cleanup

* fixed api/documents GET to exclude subrecipient and project records

* Hide download button on closed periods

* On upload, save subrecipients to subrecipients table, not documents table.

* Added subrecipient tests and cleaned up the fixtures for the other tests to only trigger the intended error

* Remove Edit button from subrecipients that have been reported to Treasury
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/data-certification/EOHHS-075-09302020-no-reviewer-v1.xlsx
+++ b/tests/server/fixtures/data-certification/EOHHS-075-09302020-no-reviewer-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/usdr/cares-reporter/tests/server/fixtures/data-certification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5518A3-9A9D-3D45-9D0B-CF883790CBA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A92F878-3B15-8242-9385-54BAA436E320}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certification" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="345">
   <si>
     <t>Certification</t>
   </si>
@@ -1081,6 +1081,9 @@
   <si>
     <t>CRF Project TOTALS</t>
   </si>
+  <si>
+    <t>A category</t>
+  </si>
 </sst>
 </file>
 
@@ -1091,7 +1094,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1150,6 +1153,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1360,7 +1369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1443,6 +1452,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7930,7 +7940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -12921,7 +12931,7 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
@@ -20095,7 +20105,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AY1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AN3" sqref="AN3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -20402,6 +20414,9 @@
         <v>9199.25</v>
       </c>
       <c r="AE3" s="14"/>
+      <c r="AN3" s="54" t="s">
+        <v>344</v>
+      </c>
       <c r="AO3" s="33">
         <v>10000</v>
       </c>
@@ -22947,7 +22962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AR1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="L1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -27688,7 +27703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="N1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -30214,7 +30229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>